<commit_message>
created functions for reading model files, func to generate simple ensemble
</commit_message>
<xml_diff>
--- a/log_book.xlsx
+++ b/log_book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barka\Desktop\big_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3D95DC-C26C-4BB0-8F52-C51191B4CB5D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F4E33B3-3232-4412-BD47-159BA0ECC07F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="86">
   <si>
     <t>Description</t>
   </si>
@@ -221,9 +221,6 @@
     <t>16/03/2020</t>
   </si>
   <si>
-    <t>week3</t>
-  </si>
-  <si>
     <t>week4</t>
   </si>
   <si>
@@ -258,6 +255,36 @@
   </si>
   <si>
     <t>Use this knowledge to build algorithms</t>
+  </si>
+  <si>
+    <t>Create separate functions to show nc file specs</t>
+  </si>
+  <si>
+    <t>31/01/2020</t>
+  </si>
+  <si>
+    <t>Create separate functions to read nc models by name or by id 1-7 or all models at once</t>
+  </si>
+  <si>
+    <t>Functions are defined in separate files</t>
+  </si>
+  <si>
+    <t>Needed to read docs for splitting functions in files</t>
+  </si>
+  <si>
+    <t>Needed to read docs about matlab functions</t>
+  </si>
+  <si>
+    <t>Explore nc files contents</t>
+  </si>
+  <si>
+    <t>Use functions models where needed</t>
+  </si>
+  <si>
+    <t>Analyze lecturer's mail related to sub-project 3. Compare the traditional ensemble with CBE</t>
+  </si>
+  <si>
+    <t>LECTURE:</t>
   </si>
 </sst>
 </file>
@@ -474,7 +501,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -529,6 +556,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Blogas" xfId="2" builtinId="27"/>
@@ -814,14 +845,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5DEC76-0ACD-4483-B15E-C162BFA7C5A1}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.77734375" customWidth="1"/>
+    <col min="5" max="5" width="41.33203125" customWidth="1"/>
     <col min="6" max="6" width="38.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35.77734375" customWidth="1"/>
     <col min="8" max="8" width="40.77734375" bestFit="1" customWidth="1"/>
@@ -833,7 +864,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>36</v>
@@ -932,7 +963,7 @@
         <v>47</v>
       </c>
       <c r="F6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
@@ -1000,7 +1031,7 @@
       </c>
       <c r="D11" s="24"/>
       <c r="E11" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1014,32 +1045,92 @@
         <v>48</v>
       </c>
       <c r="E12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F12" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" t="s">
         <v>75</v>
       </c>
-      <c r="G12" t="s">
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="25">
+        <v>43863</v>
+      </c>
+      <c r="D13" s="26">
+        <v>43863</v>
+      </c>
+      <c r="E13" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>64</v>
-      </c>
-      <c r="B25" s="25">
+      <c r="F13" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="25">
+        <v>43863</v>
+      </c>
+      <c r="D14" s="26">
+        <v>43863</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" t="s">
+        <v>83</v>
+      </c>
+      <c r="H14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B15" s="25">
+        <v>43863</v>
+      </c>
+      <c r="C15" s="25">
+        <v>43863</v>
+      </c>
+      <c r="D15" s="26">
+        <v>43863</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="25">
         <v>43892</v>
       </c>
-      <c r="C25" s="25">
+      <c r="C16" s="25">
         <v>43892</v>
       </c>
-      <c r="D25" s="25">
+      <c r="D16" s="26">
         <v>43892</v>
+      </c>
+      <c r="E16" s="27" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B26" s="25">
         <v>44106</v>
@@ -1053,7 +1144,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B27" t="s">
         <v>61</v>
@@ -1067,7 +1158,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B28" t="s">
         <v>62</v>
@@ -1081,7 +1172,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B29" s="25">
         <v>43864</v>
@@ -1095,7 +1186,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B30" s="25">
         <v>44077</v>
@@ -1109,7 +1200,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B31" t="s">
         <v>63</v>
@@ -1123,6 +1214,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
ddc algorithm downloaded from moodle
</commit_message>
<xml_diff>
--- a/log_book.xlsx
+++ b/log_book.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barka\Desktop\big_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barka\Desktop\ab\big_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F4E33B3-3232-4412-BD47-159BA0ECC07F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC6B85D-8A8F-4629-A706-A4FA169B9F2A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="90">
   <si>
     <t>Description</t>
   </si>
@@ -284,7 +284,19 @@
     <t>Analyze lecturer's mail related to sub-project 3. Compare the traditional ensemble with CBE</t>
   </si>
   <si>
-    <t>LECTURE:</t>
+    <t>Learn to measure execution time in matlab</t>
+  </si>
+  <si>
+    <t>LECTURE: code planning</t>
+  </si>
+  <si>
+    <t>I stayed till the end without break. Find out that I can use clutering to define which model is closiest to average(mean)</t>
+  </si>
+  <si>
+    <t>Map the matrix indexes to coordinates when drawing the plot</t>
+  </si>
+  <si>
+    <t>Save ensemble to simple mean file</t>
   </si>
 </sst>
 </file>
@@ -845,8 +857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5DEC76-0ACD-4483-B15E-C162BFA7C5A1}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1114,7 +1126,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B16" s="25">
         <v>43892</v>
       </c>
@@ -1125,10 +1137,40 @@
         <v>43892</v>
       </c>
       <c r="E16" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="25">
+        <v>43892</v>
+      </c>
+      <c r="E17" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B18" s="25">
+        <v>43892</v>
+      </c>
+      <c r="C18" s="25">
+        <v>43892</v>
+      </c>
+      <c r="D18" s="25">
+        <v>43892</v>
+      </c>
+      <c r="E18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>64</v>
       </c>
@@ -1142,7 +1184,7 @@
         <v>44106</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>65</v>
       </c>
@@ -1156,7 +1198,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>66</v>
       </c>
@@ -1170,7 +1212,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>67</v>
       </c>
@@ -1184,7 +1226,7 @@
         <v>43864</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>68</v>
       </c>
@@ -1198,7 +1240,7 @@
         <v>44077</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>69</v>
       </c>
@@ -1223,7 +1265,7 @@
   <dimension ref="A3:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
flowchart created, mean ensemble non-parallel function added, mapping code examples, function to get mapped coordinates
</commit_message>
<xml_diff>
--- a/log_book.xlsx
+++ b/log_book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barka\Desktop\ab\big_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC6B85D-8A8F-4629-A706-A4FA169B9F2A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDCECB9-CA6E-4679-8667-7D94381979C5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="102">
   <si>
     <t>Description</t>
   </si>
@@ -212,33 +212,6 @@
     <t>Download and fill specifiations document</t>
   </si>
   <si>
-    <t>17/02/2020</t>
-  </si>
-  <si>
-    <t>24/02/2020</t>
-  </si>
-  <si>
-    <t>16/03/2020</t>
-  </si>
-  <si>
-    <t>week4</t>
-  </si>
-  <si>
-    <t>week5</t>
-  </si>
-  <si>
-    <t>week6</t>
-  </si>
-  <si>
-    <t>week7</t>
-  </si>
-  <si>
-    <t>week8</t>
-  </si>
-  <si>
-    <t>week9</t>
-  </si>
-  <si>
     <t>Read articles about big data techniques and try to write some code</t>
   </si>
   <si>
@@ -297,12 +270,78 @@
   </si>
   <si>
     <t>Save ensemble to simple mean file</t>
+  </si>
+  <si>
+    <t>Create visualization function to plot heatmap on europe</t>
+  </si>
+  <si>
+    <t>Use it to display observations and ensembles</t>
+  </si>
+  <si>
+    <t>Analyze DDC algorithm, understand its inputs and outpus and play with it</t>
+  </si>
+  <si>
+    <t>Is the return value related to CBE?</t>
+  </si>
+  <si>
+    <t>LECTURE: code planning (different group)</t>
+  </si>
+  <si>
+    <t>I have a good idea about the project, but many tasks are waiting to be done</t>
+  </si>
+  <si>
+    <t>Had a great talk with a lecturer. Visualized my idea, found out the difference between CBE and DDC relations. Realised that given CBE data is normalized (x10^-8 is taken out from org data)</t>
+  </si>
+  <si>
+    <t>Wrote down on paper what mmajor steps will be made</t>
+  </si>
+  <si>
+    <t>Format those steps into tasks and supplement this doc with tasks</t>
+  </si>
+  <si>
+    <t>Took me a long time. I am a bit behind with this task</t>
+  </si>
+  <si>
+    <t>I had to read coordinates from the data file and pass it to a plot function</t>
+  </si>
+  <si>
+    <t>Now heat map plots LON LAT values, instead of 1-400x1-700</t>
+  </si>
+  <si>
+    <t>07/02/2020</t>
+  </si>
+  <si>
+    <t>04/02/2020</t>
+  </si>
+  <si>
+    <t>Transform my sequential simple mean ensemble function to parallel processed. Includes data deviding into subsets. Create flowchart, PSEUDOCODE</t>
+  </si>
+  <si>
+    <t>Create a flowchart</t>
+  </si>
+  <si>
+    <t>Create Pseudocode examples</t>
+  </si>
+  <si>
+    <t>10/02/2020</t>
+  </si>
+  <si>
+    <t>First try flowchart created with draw.io software</t>
+  </si>
+  <si>
+    <t>You this chart to create the code. Once code is created, write pseudocode</t>
+  </si>
+  <si>
+    <t>Hard to find good software to draw (time-consuming)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+  </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -513,7 +552,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -562,16 +601,28 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Blogas" xfId="2" builtinId="27"/>
@@ -855,18 +906,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5DEC76-0ACD-4483-B15E-C162BFA7C5A1}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="B1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.33203125" customWidth="1"/>
-    <col min="6" max="6" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.77734375" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.77734375" customWidth="1"/>
+    <col min="6" max="6" width="48" customWidth="1"/>
+    <col min="7" max="7" width="39.88671875" customWidth="1"/>
     <col min="8" max="8" width="40.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -876,7 +929,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>36</v>
@@ -895,13 +948,13 @@
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="26" t="s">
         <v>37</v>
       </c>
       <c r="E3" s="20" t="s">
@@ -916,13 +969,13 @@
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+      <c r="B4" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="28" t="s">
         <v>40</v>
       </c>
       <c r="E4" t="s">
@@ -939,13 +992,13 @@
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+      <c r="B5" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="28" t="s">
         <v>40</v>
       </c>
       <c r="E5" t="s">
@@ -962,42 +1015,53 @@
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+      <c r="B6" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="28" t="s">
         <v>48</v>
       </c>
       <c r="E6" t="s">
         <v>47</v>
       </c>
       <c r="F6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B7" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="24"/>
+      <c r="D7" s="28">
+        <v>44014</v>
+      </c>
       <c r="E7" t="s">
         <v>50</v>
       </c>
+      <c r="F7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+      <c r="B8" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="28" t="s">
         <v>49</v>
       </c>
       <c r="E8" s="21" t="s">
@@ -1011,252 +1075,272 @@
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
+      <c r="B9" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="24"/>
+      <c r="D9" s="29"/>
       <c r="E9" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+      <c r="B10" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="D10" s="24"/>
+      <c r="D10" s="29"/>
       <c r="E10" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
+      <c r="B11" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="24"/>
+      <c r="D11" s="29"/>
       <c r="E11" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B12" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="27">
+        <v>43863</v>
+      </c>
+      <c r="D13" s="28">
+        <v>43863</v>
+      </c>
+      <c r="E13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="G13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B14" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="27">
+        <v>43863</v>
+      </c>
+      <c r="D14" s="28">
+        <v>43863</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" t="s">
+        <v>74</v>
+      </c>
+      <c r="H14" t="s">
         <v>71</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G12" t="s">
+    </row>
+    <row r="15" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B15" s="27">
+        <v>43863</v>
+      </c>
+      <c r="C15" s="27">
+        <v>43863</v>
+      </c>
+      <c r="D15" s="28">
+        <v>43863</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
+    <row r="16" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B16" s="27">
+        <v>43892</v>
+      </c>
+      <c r="C16" s="27">
+        <v>43892</v>
+      </c>
+      <c r="D16" s="28">
+        <v>43892</v>
+      </c>
+      <c r="E16" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="C13" s="25">
-        <v>43863</v>
-      </c>
-      <c r="D13" s="26">
-        <v>43863</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="F16" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B17" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="29"/>
+      <c r="E18" t="s">
         <v>76</v>
       </c>
-      <c r="F13" t="s">
+    </row>
+    <row r="19" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B19" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G13" t="s">
+      <c r="F19" t="s">
+        <v>92</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B20" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="E20" t="s">
+        <v>96</v>
+      </c>
+      <c r="F20" t="s">
+        <v>99</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="24"/>
+      <c r="D21" s="31"/>
+      <c r="E21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B30" s="22">
+        <v>43953</v>
+      </c>
+      <c r="E30" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B31" s="22">
+        <v>43953</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G31" t="s">
         <v>82</v>
       </c>
-      <c r="H13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>77</v>
-      </c>
-      <c r="C14" s="25">
-        <v>43863</v>
-      </c>
-      <c r="D14" s="26">
-        <v>43863</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F14" t="s">
-        <v>79</v>
-      </c>
-      <c r="G14" t="s">
+    </row>
+    <row r="32" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B32" s="22">
+        <v>43953</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="H14" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B15" s="25">
-        <v>43863</v>
-      </c>
-      <c r="C15" s="25">
-        <v>43863</v>
-      </c>
-      <c r="D15" s="26">
-        <v>43863</v>
-      </c>
-      <c r="E15" s="1" t="s">
+      <c r="H32" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B16" s="25">
-        <v>43892</v>
-      </c>
-      <c r="C16" s="25">
-        <v>43892</v>
-      </c>
-      <c r="D16" s="26">
-        <v>43892</v>
-      </c>
-      <c r="E16" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="25">
-        <v>43892</v>
-      </c>
-      <c r="E17" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="25">
-        <v>43892</v>
-      </c>
-      <c r="C18" s="25">
-        <v>43892</v>
-      </c>
-      <c r="D18" s="25">
-        <v>43892</v>
-      </c>
-      <c r="E18" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E19" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>64</v>
-      </c>
-      <c r="B26" s="25">
-        <v>44106</v>
-      </c>
-      <c r="C26" s="25">
-        <v>44106</v>
-      </c>
-      <c r="D26" s="25">
-        <v>44106</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>65</v>
-      </c>
-      <c r="B27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" t="s">
-        <v>61</v>
-      </c>
-      <c r="D27" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>66</v>
-      </c>
-      <c r="B28" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" t="s">
-        <v>62</v>
-      </c>
-      <c r="D28" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>67</v>
-      </c>
-      <c r="B29" s="25">
-        <v>43864</v>
-      </c>
-      <c r="C29" s="25">
-        <v>43864</v>
-      </c>
-      <c r="D29" s="25">
-        <v>43864</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>68</v>
-      </c>
-      <c r="B30" s="25">
-        <v>44077</v>
-      </c>
-      <c r="C30" s="25">
-        <v>44077</v>
-      </c>
-      <c r="D30" s="25">
-        <v>44077</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>69</v>
-      </c>
-      <c r="B31" t="s">
-        <v>63</v>
-      </c>
-      <c r="C31" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
logbook updated, specifications finished, sample scripts added
</commit_message>
<xml_diff>
--- a/log_book.xlsx
+++ b/log_book.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barka\Desktop\ab\big_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barka\Desktop\uni\5011\big-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDCECB9-CA6E-4679-8667-7D94381979C5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6077C45D-12C3-4169-AE8B-3933C8A5C830}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-9360" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Work plan" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="133">
   <si>
     <t>Description</t>
   </si>
@@ -269,33 +269,15 @@
     <t>Map the matrix indexes to coordinates when drawing the plot</t>
   </si>
   <si>
-    <t>Save ensemble to simple mean file</t>
-  </si>
-  <si>
-    <t>Create visualization function to plot heatmap on europe</t>
-  </si>
-  <si>
-    <t>Use it to display observations and ensembles</t>
-  </si>
-  <si>
     <t>Analyze DDC algorithm, understand its inputs and outpus and play with it</t>
   </si>
   <si>
-    <t>Is the return value related to CBE?</t>
-  </si>
-  <si>
-    <t>LECTURE: code planning (different group)</t>
-  </si>
-  <si>
     <t>I have a good idea about the project, but many tasks are waiting to be done</t>
   </si>
   <si>
     <t>Had a great talk with a lecturer. Visualized my idea, found out the difference between CBE and DDC relations. Realised that given CBE data is normalized (x10^-8 is taken out from org data)</t>
   </si>
   <si>
-    <t>Wrote down on paper what mmajor steps will be made</t>
-  </si>
-  <si>
     <t>Format those steps into tasks and supplement this doc with tasks</t>
   </si>
   <si>
@@ -326,13 +308,124 @@
     <t>10/02/2020</t>
   </si>
   <si>
-    <t>First try flowchart created with draw.io software</t>
-  </si>
-  <si>
     <t>You this chart to create the code. Once code is created, write pseudocode</t>
   </si>
   <si>
     <t>Hard to find good software to draw (time-consuming)</t>
+  </si>
+  <si>
+    <t>11/02/2020</t>
+  </si>
+  <si>
+    <t>Its just 2 commands needed: tic and toc</t>
+  </si>
+  <si>
+    <t>implement some sequential and parallel processign and compare results</t>
+  </si>
+  <si>
+    <t>Use flowchart to create tasks in logbook</t>
+  </si>
+  <si>
+    <t>LECTURE: code planning (other group)</t>
+  </si>
+  <si>
+    <t>05/02/2020</t>
+  </si>
+  <si>
+    <t>06/02/2020</t>
+  </si>
+  <si>
+    <t>02/02/2020</t>
+  </si>
+  <si>
+    <t>Analyze moodle code for parallel processing, make notes</t>
+  </si>
+  <si>
+    <t>Analyze moodle code for figure drawing and make some notes</t>
+  </si>
+  <si>
+    <t>Some unexpeted delays due to the lack of fundamental matlab knowledge</t>
+  </si>
+  <si>
+    <t>Generate README page including: installation guide, folder/file description, idea explanation, output examples</t>
+  </si>
+  <si>
+    <t>This simple README guide lets quickly descripbe this project for people involved in it</t>
+  </si>
+  <si>
+    <t>After some time, don’t forget to improve it as things change quite often</t>
+  </si>
+  <si>
+    <t>Matlab doesn’t support MD files</t>
+  </si>
+  <si>
+    <t>Transform CBE from .csv files to .mat</t>
+  </si>
+  <si>
+    <t>Implement parallel processed simple mean ensemble algorithm (add func param: saveToFile: bool)</t>
+  </si>
+  <si>
+    <t>Write a function to load ensembles: CBE or SME (add parameter to determine which one) where data is saved in "/data/x.mat" file</t>
+  </si>
+  <si>
+    <t>Ask teacher what he means by: "compare CBE/SME (bias) with the observations"</t>
+  </si>
+  <si>
+    <t>Write an algorithm to calculate difference (bias) between CBE and SME SEQUENTIALY</t>
+  </si>
+  <si>
+    <t>Write an algorithm to calculate difference (bias) between CBE and SME in PARALLEL</t>
+  </si>
+  <si>
+    <t>Write a function to draw a Ozone map in Europe region where args are: ensemble/model</t>
+  </si>
+  <si>
+    <t>Save observation figures to file (expected 3)</t>
+  </si>
+  <si>
+    <t>Wrote down on paper what major steps will be made</t>
+  </si>
+  <si>
+    <t>Reflect my project specification with a friend and lecturer</t>
+  </si>
+  <si>
+    <t>14/02/2020</t>
+  </si>
+  <si>
+    <t>DDC return value (points assigned to clusters) is beeing used to calculate a CBE</t>
+  </si>
+  <si>
+    <t>19/01/2020</t>
+  </si>
+  <si>
+    <t>This task required the most time to complete</t>
+  </si>
+  <si>
+    <t>Ask for feedback from the turor</t>
+  </si>
+  <si>
+    <t>Specifications document is created</t>
+  </si>
+  <si>
+    <t>17/02/2020</t>
+  </si>
+  <si>
+    <t>16/02/2020</t>
+  </si>
+  <si>
+    <t>Flowchart made in .project and .jpg formats</t>
+  </si>
+  <si>
+    <t>Tasks were added down below</t>
+  </si>
+  <si>
+    <t>Finish the tasks before the separator line and then continue</t>
+  </si>
+  <si>
+    <t>Now I understand how I can create parallel processing. PAR is faster</t>
+  </si>
+  <si>
+    <t>There is advanced Parallel processing which can win so extra time compared to regular parallel processing</t>
   </si>
 </sst>
 </file>
@@ -427,7 +520,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -545,6 +638,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -552,7 +654,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -560,7 +662,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -582,9 +683,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -601,7 +699,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -618,11 +715,40 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="9" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Blogas" xfId="2" builtinId="27"/>
@@ -641,6 +767,75 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>76201</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>328189</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Paveikslėlis 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{472483EB-14EB-4A9C-A25F-7441E7B33971}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7452361" y="373380"/>
+          <a:ext cx="4046748" cy="6560820"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100" cap="sq">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -906,18 +1101,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5DEC76-0ACD-4483-B15E-C162BFA7C5A1}">
-  <dimension ref="B1:H32"/>
+  <dimension ref="B1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="34" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.77734375" customWidth="1"/>
+    <col min="5" max="5" width="44.44140625" customWidth="1"/>
     <col min="6" max="6" width="48" customWidth="1"/>
     <col min="7" max="7" width="39.88671875" customWidth="1"/>
     <col min="8" max="8" width="40.77734375" bestFit="1" customWidth="1"/>
@@ -925,57 +1120,57 @@
   <sheetData>
     <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="16" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19" t="s">
+      <c r="F3" s="17"/>
+      <c r="G3" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="17" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="25" t="s">
         <v>40</v>
       </c>
       <c r="E4" t="s">
@@ -992,13 +1187,13 @@
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="25" t="s">
         <v>40</v>
       </c>
       <c r="E5" t="s">
@@ -1015,10 +1210,10 @@
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="24" t="s">
         <v>54</v>
       </c>
       <c r="D6" s="28" t="s">
@@ -1032,39 +1227,39 @@
       </c>
     </row>
     <row r="7" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="28">
-        <v>44014</v>
+      <c r="D7" s="26" t="s">
+        <v>54</v>
       </c>
       <c r="E7" t="s">
         <v>50</v>
       </c>
       <c r="F7" t="s">
-        <v>88</v>
+        <v>118</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="24" t="s">
         <v>49</v>
       </c>
       <c r="D8" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="19" t="s">
         <v>55</v>
       </c>
       <c r="G8" t="s">
@@ -1074,35 +1269,49 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="27" t="s">
+    <row r="9" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B9" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="24" t="s">
         <v>59</v>
       </c>
       <c r="D9" s="29"/>
       <c r="E9" t="s">
         <v>58</v>
       </c>
+      <c r="H9" s="1" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="D10" s="29"/>
+      <c r="D10" s="28" t="s">
+        <v>122</v>
+      </c>
       <c r="E10" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="27" t="s">
+      <c r="F10" t="s">
+        <v>125</v>
+      </c>
+      <c r="G10" t="s">
+        <v>124</v>
+      </c>
+      <c r="H10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="24" t="s">
         <v>48</v>
       </c>
       <c r="D11" s="29"/>
@@ -1111,10 +1320,10 @@
       </c>
     </row>
     <row r="12" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="24" t="s">
         <v>48</v>
       </c>
       <c r="D12" s="28" t="s">
@@ -1131,14 +1340,14 @@
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="27">
-        <v>43863</v>
-      </c>
-      <c r="D13" s="28">
-        <v>43863</v>
+      <c r="C13" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>100</v>
       </c>
       <c r="E13" t="s">
         <v>67</v>
@@ -1154,14 +1363,14 @@
       </c>
     </row>
     <row r="14" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="27">
-        <v>43863</v>
-      </c>
-      <c r="D14" s="28">
-        <v>43863</v>
+      <c r="C14" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>100</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>69</v>
@@ -1177,30 +1386,30 @@
       </c>
     </row>
     <row r="15" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B15" s="27">
-        <v>43863</v>
-      </c>
-      <c r="C15" s="27">
-        <v>43863</v>
-      </c>
-      <c r="D15" s="28">
-        <v>43863</v>
+      <c r="B15" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>101</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B16" s="27">
-        <v>43892</v>
-      </c>
-      <c r="C16" s="27">
-        <v>43892</v>
-      </c>
-      <c r="D16" s="28">
-        <v>43892</v>
-      </c>
-      <c r="E16" s="23" t="s">
+      <c r="B16" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="E16" s="20" t="s">
         <v>77</v>
       </c>
       <c r="F16" s="1" t="s">
@@ -1208,135 +1417,276 @@
       </c>
     </row>
     <row r="17" spans="2:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B17" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="C17" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="D17" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>85</v>
+      <c r="B17" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>99</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G17" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B18" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="29"/>
       <c r="E18" t="s">
         <v>76</v>
       </c>
+      <c r="F18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="19" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B19" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="C19" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="D19" s="30" t="s">
-        <v>94</v>
+      <c r="B19" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>88</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>79</v>
       </c>
       <c r="F19" t="s">
+        <v>86</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B20" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="C20" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" t="s">
+        <v>90</v>
+      </c>
+      <c r="F20" t="s">
+        <v>128</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="21"/>
+      <c r="D21" s="27"/>
+      <c r="E21" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B20" s="27" t="s">
+    <row r="22" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B22" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="D22" s="41" t="s">
+        <v>126</v>
+      </c>
+      <c r="E22" t="s">
         <v>98</v>
       </c>
-      <c r="C20" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="D20" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="E20" t="s">
-        <v>96</v>
-      </c>
-      <c r="F20" t="s">
-        <v>99</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="31"/>
-      <c r="E21" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
+      <c r="F22" t="s">
+        <v>129</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B23" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D23" s="41" t="s">
+        <v>126</v>
+      </c>
+      <c r="E23" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B24" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="C24" s="21"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B25" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="D25" s="36">
+        <v>44137</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B30" s="22">
-        <v>43953</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="B26" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="37"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+    </row>
+    <row r="27" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" s="27"/>
+      <c r="E27" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B28" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" s="27"/>
+      <c r="E28" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B29" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" s="27"/>
+      <c r="E29" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B30" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" s="27"/>
+      <c r="E30" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B31" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="D31" s="27"/>
+      <c r="E31" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B32" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" s="27"/>
+      <c r="E32" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B33" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="D33" s="27"/>
+      <c r="E33" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B34" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34" t="s">
+        <v>120</v>
+      </c>
+      <c r="D34" s="27"/>
+      <c r="E34" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B35" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="D35" s="27"/>
+      <c r="E35" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="31" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B31" s="22">
-        <v>43953</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G31" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B32" s="22">
-        <v>43953</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H32" t="s">
-        <v>84</v>
-      </c>
+      <c r="F35" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E42" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1349,7 +1699,7 @@
   <dimension ref="A3:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1406,10 +1756,10 @@
       <c r="A16" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="12" t="s">
         <v>26</v>
       </c>
       <c r="D16" t="s">
@@ -1431,7 +1781,7 @@
       <c r="B18" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="12" t="s">
         <v>30</v>
       </c>
       <c r="D18" t="s">
@@ -1452,7 +1802,7 @@
   <dimension ref="B2:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1465,57 +1815,57 @@
   <sheetData>
     <row r="2" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="32" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="32" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1543,5 +1893,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Logbook updates, new flowchart dist/index.m file loads necessarily data SME, CBE and Observations Models scaling method appended
</commit_message>
<xml_diff>
--- a/log_book.xlsx
+++ b/log_book.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barka\Desktop\uni\5011\big-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6077C45D-12C3-4169-AE8B-3933C8A5C830}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839882CE-4709-4CE8-9C38-2AE8AEAC6712}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-9360" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Work plan" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="166">
   <si>
     <t>Description</t>
   </si>
@@ -371,18 +371,6 @@
     <t>Ask teacher what he means by: "compare CBE/SME (bias) with the observations"</t>
   </si>
   <si>
-    <t>Write an algorithm to calculate difference (bias) between CBE and SME SEQUENTIALY</t>
-  </si>
-  <si>
-    <t>Write an algorithm to calculate difference (bias) between CBE and SME in PARALLEL</t>
-  </si>
-  <si>
-    <t>Write a function to draw a Ozone map in Europe region where args are: ensemble/model</t>
-  </si>
-  <si>
-    <t>Save observation figures to file (expected 3)</t>
-  </si>
-  <si>
     <t>Wrote down on paper what major steps will be made</t>
   </si>
   <si>
@@ -426,6 +414,117 @@
   </si>
   <si>
     <t>There is advanced Parallel processing which can win so extra time compared to regular parallel processing</t>
+  </si>
+  <si>
+    <t>20/02/2020</t>
+  </si>
+  <si>
+    <t>Sectionize the index file by %% comments using flowchat to facilitate code readibility</t>
+  </si>
+  <si>
+    <t>21/02/2020</t>
+  </si>
+  <si>
+    <t>LECTURE: project development</t>
+  </si>
+  <si>
+    <t>Lecturer explained how Data Density algorithm works and how to use the results to generate CBE. Loaded 3 different models into matlab: CBE (scaling was used), SME and Observatiosns. Found out that Orig files given by teacher are different from my generated SME and this is potentially an Observations data which I am going to use as well to show that CBE is more accurate compared to SME</t>
+  </si>
+  <si>
+    <t>Use SME, CBE and Observations to calculate biases. Also, generate new flowchart due to fact updates (Orig is possibly an Observations data)</t>
+  </si>
+  <si>
+    <t>Orig data files are quite different compared to the generated mean ensemble by myself. This bring a little comfusion. I am going to assume that Orig data is Observations and use it in my project, which makes the project more difficult as I have to handle more data</t>
+  </si>
+  <si>
+    <t>Refactor Data Flow Diagram</t>
+  </si>
+  <si>
+    <t>22/02/2020</t>
+  </si>
+  <si>
+    <t>DFD can be found in images directory named flowchart2.png</t>
+  </si>
+  <si>
+    <t>Use updated DFD to create code, refactor tasks</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Answered the question on 21/02/2020. Observation is the real measurments that were used to prove that data clustering is more accurate than mean model</t>
+  </si>
+  <si>
+    <t>Lack of definions in module introduction dragged my progress a bit down as I was unable to develop</t>
+  </si>
+  <si>
+    <t>No difficulties</t>
+  </si>
+  <si>
+    <t>DFD changed</t>
+  </si>
+  <si>
+    <t>Load Observation values from /data/org</t>
+  </si>
+  <si>
+    <t>Load 7 models and calc SME (mean)</t>
+  </si>
+  <si>
+    <t>Data loaded into var SME</t>
+  </si>
+  <si>
+    <t>Data loaded into var ORG</t>
+  </si>
+  <si>
+    <t>Load CBE values from /data/cbe</t>
+  </si>
+  <si>
+    <t>Data loaded into var CBE</t>
+  </si>
+  <si>
+    <t>use to calculate bias with ORG</t>
+  </si>
+  <si>
+    <t>Parallel processing takes more time than sequential, possibly due to small data set</t>
+  </si>
+  <si>
+    <t>Comments added to make code sections which helps to indentify which flowchart part it belongs to</t>
+  </si>
+  <si>
+    <t>Start implementing the code - flowchart</t>
+  </si>
+  <si>
+    <t>Parallel processing is inefficient to use with small data set</t>
+  </si>
+  <si>
+    <t>Time measuarments (tic,toc) shows that sequential code is faster</t>
+  </si>
+  <si>
+    <t>Write an algorithm to calculate difference (bias) between ORG and SME (in parallel)</t>
+  </si>
+  <si>
+    <t>Write an algorithm to calculate difference (bias) between ORG and CBE (in parallel)</t>
+  </si>
+  <si>
+    <t>Write a function to draw a Ozone map in Europe region where args are: matrix/model 698x398</t>
+  </si>
+  <si>
+    <t>Improve map plot by adding coordinate Axis values, and title</t>
+  </si>
+  <si>
+    <t>Save observation figures to file (expected 5)</t>
+  </si>
+  <si>
+    <t>Lecturer took a look, positive review</t>
+  </si>
+  <si>
+    <t>Develop the code</t>
+  </si>
+  <si>
+    <t>My project doesn't involve using DDC algorithm. I get CBE model by itself</t>
+  </si>
+  <si>
+    <t>Clean up the data files (remove unused), clean up the code</t>
   </si>
 </sst>
 </file>
@@ -435,7 +534,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -501,8 +600,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -519,6 +625,11 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -641,20 +752,21 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -739,22 +851,45 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="4"/>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="9" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="9" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Blogas" xfId="2" builtinId="27"/>
     <cellStyle name="Geras" xfId="1" builtinId="26"/>
     <cellStyle name="Hipersaitas" xfId="3" builtinId="8"/>
     <cellStyle name="Įprastas" xfId="0" builtinId="0"/>
+    <cellStyle name="Neutralus" xfId="4" builtinId="28"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1101,21 +1236,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5DEC76-0ACD-4483-B15E-C162BFA7C5A1}">
-  <dimension ref="B1:H42"/>
+  <dimension ref="B1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="1" max="1" width="2.109375" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" style="34" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.44140625" customWidth="1"/>
-    <col min="6" max="6" width="48" customWidth="1"/>
-    <col min="7" max="7" width="39.88671875" customWidth="1"/>
-    <col min="8" max="8" width="40.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.33203125" customWidth="1"/>
+    <col min="6" max="6" width="50.44140625" customWidth="1"/>
+    <col min="7" max="7" width="35.88671875" customWidth="1"/>
+    <col min="8" max="8" width="38" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1240,7 +1375,7 @@
         <v>50</v>
       </c>
       <c r="F7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>83</v>
@@ -1276,7 +1411,7 @@
       <c r="C9" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="29"/>
+      <c r="D9" s="45"/>
       <c r="E9" t="s">
         <v>58</v>
       </c>
@@ -1292,19 +1427,19 @@
         <v>59</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E10" t="s">
         <v>60</v>
       </c>
       <c r="F10" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="G10" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="H10" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -1493,7 +1628,7 @@
         <v>90</v>
       </c>
       <c r="F20" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>93</v>
@@ -1507,7 +1642,7 @@
         <v>92</v>
       </c>
       <c r="C21" s="21"/>
-      <c r="D21" s="27"/>
+      <c r="D21" s="44"/>
       <c r="E21" t="s">
         <v>91</v>
       </c>
@@ -1517,19 +1652,19 @@
         <v>95</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="D22" s="41" t="s">
-        <v>126</v>
+        <v>123</v>
+      </c>
+      <c r="D22" s="36" t="s">
+        <v>122</v>
       </c>
       <c r="E22" t="s">
         <v>98</v>
       </c>
       <c r="F22" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1537,19 +1672,19 @@
         <v>95</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="D23" s="41" t="s">
-        <v>126</v>
+        <v>122</v>
+      </c>
+      <c r="D23" s="36" t="s">
+        <v>122</v>
       </c>
       <c r="E23" s="33" t="s">
         <v>103</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1557,136 +1692,339 @@
         <v>95</v>
       </c>
       <c r="C24" s="21"/>
-      <c r="D24" s="27"/>
+      <c r="D24" s="44"/>
       <c r="E24" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B25" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="D25" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G25" t="s">
+        <v>154</v>
+      </c>
+      <c r="H25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="C25" s="24" t="s">
+      <c r="C26" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="D25" s="36">
+      <c r="D26" s="47">
         <v>44137</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E26" s="48" t="s">
         <v>106</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F26" s="48" t="s">
         <v>107</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G26" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="H26" s="48" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="39" t="s">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="C26" s="37"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="38" t="s">
+      <c r="C27" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="D27" s="42" t="s">
+        <v>140</v>
+      </c>
+      <c r="E27" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="F26" s="38"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
-    </row>
-    <row r="27" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="34" t="s">
+      <c r="F27" s="43" t="s">
+        <v>144</v>
+      </c>
+      <c r="G27" s="43"/>
+      <c r="H27" s="43"/>
+    </row>
+    <row r="28" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>137</v>
+      </c>
+      <c r="C28" t="s">
+        <v>137</v>
+      </c>
+      <c r="D28" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F28" t="s">
+        <v>147</v>
+      </c>
+      <c r="G28" t="s">
+        <v>151</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>137</v>
+      </c>
+      <c r="C29" t="s">
+        <v>137</v>
+      </c>
+      <c r="D29" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F29" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>137</v>
+      </c>
+      <c r="C30" t="s">
+        <v>137</v>
+      </c>
+      <c r="D30" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F30" t="s">
+        <v>150</v>
+      </c>
+      <c r="G30" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="D27" s="27"/>
-      <c r="E27" s="1" t="s">
+      <c r="C31" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="D31" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="E31" s="39" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="28" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B28" s="34" t="s">
+      <c r="F31" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+    </row>
+    <row r="32" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B32" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="D28" s="27"/>
-      <c r="E28" s="1" t="s">
+      <c r="C32" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="D32" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="E32" s="39" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="29" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B29" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="D29" s="27"/>
-      <c r="E29" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B30" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="D30" s="27"/>
-      <c r="E30" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B31" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="D31" s="27"/>
-      <c r="E31" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B32" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="D32" s="27"/>
-      <c r="E32" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F32" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="G32" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="H32" s="27"/>
+    </row>
+    <row r="33" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B33" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="D33" s="27"/>
+      <c r="C33" s="40">
+        <v>44167</v>
+      </c>
+      <c r="D33" s="36" t="s">
+        <v>131</v>
+      </c>
       <c r="E33" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B34" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="C34" t="s">
-        <v>120</v>
-      </c>
-      <c r="D34" s="27"/>
+      <c r="D34" s="44"/>
       <c r="E34" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B35" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="D35" s="27"/>
+      <c r="D35" s="44"/>
       <c r="E35" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B36" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="D36" s="44"/>
+      <c r="E36" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B37" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="D37" s="44"/>
+      <c r="E37" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B38" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="D38" s="44"/>
+      <c r="E38" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B39" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C39" t="s">
+        <v>116</v>
+      </c>
+      <c r="D39" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F39" t="s">
+        <v>162</v>
+      </c>
+      <c r="G39" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" s="50" t="s">
+        <v>137</v>
+      </c>
+      <c r="D40" s="50" t="s">
+        <v>140</v>
+      </c>
+      <c r="E40" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="E42" s="1"/>
+      <c r="F40" s="51" t="s">
+        <v>164</v>
+      </c>
+      <c r="G40" s="51" t="s">
+        <v>117</v>
+      </c>
+      <c r="H40" s="50"/>
+    </row>
+    <row r="41" spans="2:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B41" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="C41" t="s">
+        <v>131</v>
+      </c>
+      <c r="D41" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B42" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="C42" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="D42" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="E42" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="F42" t="s">
+        <v>138</v>
+      </c>
+      <c r="G42" t="s">
+        <v>139</v>
+      </c>
+      <c r="H42" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="D43" s="44"/>
+      <c r="E43" s="37" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="E47" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
plotting functions implemented auto save SME data implemented
</commit_message>
<xml_diff>
--- a/log_book.xlsx
+++ b/log_book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barka\Desktop\uni\5011\big-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839882CE-4709-4CE8-9C38-2AE8AEAC6712}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98CF6CB-D842-4689-B585-F7EC29111F4E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="167">
   <si>
     <t>Description</t>
   </si>
@@ -525,6 +525,9 @@
   </si>
   <si>
     <t>Clean up the data files (remove unused), clean up the code</t>
+  </si>
+  <si>
+    <t>Update readme guide to run the project</t>
   </si>
 </sst>
 </file>
@@ -1238,8 +1241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5DEC76-0ACD-4483-B15E-C162BFA7C5A1}">
   <dimension ref="B1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1841,7 +1844,7 @@
       <c r="G31" s="27"/>
       <c r="H31" s="27"/>
     </row>
-    <row r="32" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B32" s="38" t="s">
         <v>95</v>
       </c>
@@ -2021,6 +2024,15 @@
       <c r="D43" s="44"/>
       <c r="E43" s="37" t="s">
         <v>165</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B44" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="D44" s="44"/>
+      <c r="E44" s="37" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
plotting features: with slider, subplots program menu implementation functions for loading various data files
</commit_message>
<xml_diff>
--- a/log_book.xlsx
+++ b/log_book.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barka\Desktop\uni\5011\big-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98CF6CB-D842-4689-B585-F7EC29111F4E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273954E3-CE5B-4164-B643-04A964C7F237}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-9360" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Work plan" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="170">
   <si>
     <t>Description</t>
   </si>
@@ -528,6 +528,15 @@
   </si>
   <si>
     <t>Update readme guide to run the project</t>
+  </si>
+  <si>
+    <t>23/02/2020</t>
+  </si>
+  <si>
+    <t>24/02/2020</t>
+  </si>
+  <si>
+    <t>data folder now holds data in different folders for different ensembles</t>
   </si>
 </sst>
 </file>
@@ -1241,8 +1250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5DEC76-0ACD-4483-B15E-C162BFA7C5A1}">
   <dimension ref="B1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2021,9 +2030,17 @@
       <c r="B43" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="D43" s="44"/>
+      <c r="C43" t="s">
+        <v>167</v>
+      </c>
+      <c r="D43" s="36" t="s">
+        <v>168</v>
+      </c>
       <c r="E43" s="37" t="s">
         <v>165</v>
+      </c>
+      <c r="F43" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.3">

</xml_diff>